<commit_message>
edit laporan lipa 24
</commit_message>
<xml_diff>
--- a/hasil/2023_05_lipa_24.xlsx
+++ b/hasil/2023_05_lipa_24.xlsx
@@ -59,7 +59,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 10 Agustus 2023</t>
+    <t>Ternate , 22 September 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -801,7 +801,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" customHeight="1" ht="90">
+    <row r="9" spans="1:19" customHeight="1" ht="65">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -809,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9" s="18">
         <v>0</v>
@@ -824,7 +824,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>

</xml_diff>